<commit_message>
test: update test case for #62
</commit_message>
<xml_diff>
--- a/src/test/resources/org/bbreak/excella/reports/tag/ImageParamParserTest.xlsx
+++ b/src/test/resources/org/bbreak/excella/reports/tag/ImageParamParserTest.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER1\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126DE806-E813-45B3-AE37-AFAB3C4B8EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="285" windowWidth="11655" windowHeight="9285" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,8 +131,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,15 +155,21 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -165,17 +177,155 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -184,13 +334,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -228,7 +386,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -262,6 +420,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -296,9 +455,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -471,94 +631,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="4"/>
       <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="8"/>
       <c r="D6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="4"/>
       <c r="D12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="8"/>
       <c r="D15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -575,14 +735,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -590,7 +750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -599,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -607,10 +767,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -619,11 +779,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -631,7 +791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -640,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -648,10 +808,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -660,7 +820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
@@ -679,16 +839,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -696,7 +854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -705,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -713,10 +871,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -725,11 +883,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -737,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -746,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -754,10 +912,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -766,7 +924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
@@ -785,19 +943,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -805,7 +961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -813,7 +969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -821,7 +977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -836,19 +992,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -856,7 +1010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -864,7 +1018,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -872,7 +1026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
fix: The ruled lines of unmerged cells disappear
</commit_message>
<xml_diff>
--- a/src/test/resources/org/bbreak/excella/reports/tag/ImageParamParserTest.xlsx
+++ b/src/test/resources/org/bbreak/excella/reports/tag/ImageParamParserTest.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER1\git\excella-reports\src\test\resources\org\bbreak\excella\reports\tag\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C759550-F30C-4958-9833-4B89D6B5FC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="285" windowWidth="11655" windowHeight="9285" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,8 +131,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,13 +190,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -228,7 +242,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -262,6 +276,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -296,9 +311,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -471,14 +487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -486,7 +502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -495,7 +511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -503,10 +519,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -515,11 +531,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -527,7 +543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -536,7 +552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -544,10 +560,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -556,7 +572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
@@ -575,14 +591,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -590,7 +606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -599,7 +615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -607,10 +623,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -619,11 +635,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -631,7 +647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -640,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -648,10 +664,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -660,7 +676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
@@ -679,16 +695,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -696,7 +710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -705,7 +719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -713,10 +727,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -725,11 +739,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -737,7 +751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -746,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -754,10 +768,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -766,7 +780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
@@ -785,19 +799,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -805,7 +817,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -813,7 +825,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -821,7 +833,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -836,19 +848,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -856,7 +866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -864,7 +874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -872,7 +882,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
fix: sheet 1 of the ImageParamParserTest Excel files
</commit_message>
<xml_diff>
--- a/src/test/resources/org/bbreak/excella/reports/tag/ImageParamParserTest.xlsx
+++ b/src/test/resources/org/bbreak/excella/reports/tag/ImageParamParserTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER1\git\excella-reports\src\test\resources\org\bbreak\excella\reports\tag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C759550-F30C-4958-9833-4B89D6B5FC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126DE806-E813-45B3-AE37-AFAB3C4B8EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,15 +155,21 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -171,17 +177,155 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -495,7 +639,7 @@
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
@@ -503,16 +647,16 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="4"/>
       <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
@@ -520,23 +664,23 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
+      <c r="A5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="8"/>
       <c r="D6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
@@ -544,16 +688,16 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="4"/>
       <c r="D12" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
@@ -561,20 +705,20 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="1"/>
+      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="8"/>
       <c r="D15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
fix(ImageParamParser): unmerged cells' CellStyle (border line, color, etc...) disappear (#63)
* fix: The ruled lines of unmerged cells disappear

* fix: sheet 1 of the ImageParamParserTest Excel files

* 不要なコメントを削除
</commit_message>
<xml_diff>
--- a/src/test/resources/org/bbreak/excella/reports/tag/ImageParamParserTest.xlsx
+++ b/src/test/resources/org/bbreak/excella/reports/tag/ImageParamParserTest.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER1\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126DE806-E813-45B3-AE37-AFAB3C4B8EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="285" windowWidth="11655" windowHeight="9285" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,8 +131,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,15 +155,21 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -165,17 +177,155 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -184,13 +334,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -228,7 +386,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -262,6 +420,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -296,9 +455,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -471,94 +631,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="4"/>
       <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="8"/>
       <c r="D6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="4"/>
       <c r="D12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="8"/>
       <c r="D15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -575,14 +735,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -590,7 +750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -599,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -607,10 +767,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -619,11 +779,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -631,7 +791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -640,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -648,10 +808,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -660,7 +820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
@@ -679,16 +839,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -696,7 +854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -705,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -713,10 +871,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -725,11 +883,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -737,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -746,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -754,10 +912,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -766,7 +924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
@@ -785,19 +943,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -805,7 +961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -813,7 +969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -821,7 +977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -836,19 +992,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -856,7 +1010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -864,7 +1018,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -872,7 +1026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>19</v>
       </c>

</xml_diff>